<commit_message>
Adição da pesquisa de funcionalidades
</commit_message>
<xml_diff>
--- a/docs/projeto-final/documento-final/pesquisas/pesquisas.xlsx
+++ b/docs/projeto-final/documento-final/pesquisas/pesquisas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Desenvolvimento\FAI\fai.etanois.docs\docs\projeto-final\documento-final\pesquisas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.barbosa\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0DD0E0F-8043-4CFC-865C-BDCFBA2DB867}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DFCEF80-0BEC-48A7-B524-0DB884728D47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{D9E7E27E-ABC6-4427-AF05-B1E2A0954FEE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{D9E7E27E-ABC6-4427-AF05-B1E2A0954FEE}"/>
   </bookViews>
   <sheets>
     <sheet name="Pesquisa #01 - Valores" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="74">
   <si>
     <t>Pesquisa #01 - Acompanhamento dos valores dos postos de combustível</t>
   </si>
@@ -74,6 +74,186 @@
   </si>
   <si>
     <t>Quantidade de aparições</t>
+  </si>
+  <si>
+    <t>Mostrar os postos mais baratos no trecho</t>
+  </si>
+  <si>
+    <t>De 20 a 64 anos</t>
+  </si>
+  <si>
+    <t>Mostrar nota de qualidade em atendimento, loja de conveniência, limpeza de banheiro e preço</t>
+  </si>
+  <si>
+    <t>Mostrar formas de pagamento e bandeiras dos cartões de créditos aceitos</t>
+  </si>
+  <si>
+    <t>Possiblidade de interagir com loja de conveniência e abastecimento pagos por aplicativo</t>
+  </si>
+  <si>
+    <t>Mostrar os valores de cada tipo de combustível do posto, etanol, gasolina e gasolina aditivada</t>
+  </si>
+  <si>
+    <t>Criar programa diferenciado de fidelidade, que valesse para qualquer posto, independente da bandeira</t>
+  </si>
+  <si>
+    <t>Mostrar distância aproximada dos postos em relação ao motorista</t>
+  </si>
+  <si>
+    <t>Mostar as bandeiras dos postos</t>
+  </si>
+  <si>
+    <t>Mostrar as diferenças entre pagar com cartão de crédito ou a vista</t>
+  </si>
+  <si>
+    <t>Mostrar se posto possui borracheiro</t>
+  </si>
+  <si>
+    <t>Possuir roteamento do inicio até fim viagem</t>
+  </si>
+  <si>
+    <t>Registrar os abastecimentos do motorista</t>
+  </si>
+  <si>
+    <t>Registrar gastos com manutenção do carro</t>
+  </si>
+  <si>
+    <t>Registrar pagamentos IPVA</t>
+  </si>
+  <si>
+    <t>Registrar carteira de motorista do usuário</t>
+  </si>
+  <si>
+    <t>Registrar documentação do veiculo</t>
+  </si>
+  <si>
+    <t>Gerar relatórios dos gastos do usuario no mês.</t>
+  </si>
+  <si>
+    <t>Gerar relatórios de consumo médio do carro do mês</t>
+  </si>
+  <si>
+    <t>Avisar o vencimento das despesas</t>
+  </si>
+  <si>
+    <t>Avisar quando carteira e documentos do carro vencem</t>
+  </si>
+  <si>
+    <t>Mostrar os postos mais próximos do usuário</t>
+  </si>
+  <si>
+    <t>Mostrar os preços dos postos</t>
+  </si>
+  <si>
+    <t>Filtrar posto por bandeira de cartão de crédito</t>
+  </si>
+  <si>
+    <t>Mostrar resumo das rotas</t>
+  </si>
+  <si>
+    <t>Mostrar média de preço do combustível na rota</t>
+  </si>
+  <si>
+    <t>Mostrar os 4 postos abaixo da média geral</t>
+  </si>
+  <si>
+    <t>Mostrar o posto que está em promoção</t>
+  </si>
+  <si>
+    <t>Mostrar postos com denuncia combustível adulterado e marcação errada de combustível</t>
+  </si>
+  <si>
+    <t>Mostrar serviços de guincho na rota</t>
+  </si>
+  <si>
+    <t>Fazer algo parecido com quilometros de vantagem, o motorista vai ganhando algo a medida que abastece</t>
+  </si>
+  <si>
+    <t>Criar Forma de fidelizar o motorista e o posto</t>
+  </si>
+  <si>
+    <t>Calcular consumo médio do carro, de acordo com quilometragem e combustível colocado</t>
+  </si>
+  <si>
+    <t>Filtrar postos por bandeira</t>
+  </si>
+  <si>
+    <t>Informar se o posto tem lava-rápido</t>
+  </si>
+  <si>
+    <t>Informar horário de funcionamento posto</t>
+  </si>
+  <si>
+    <t>Possibilidade do usuário poder cadastrar seus postos favoritos</t>
+  </si>
+  <si>
+    <t>Possibilidade do usuário atualisar os preços dos combustíveis e ganhar pontos com isso, estes pontos poderem ser trocados por descontos nos postos</t>
+  </si>
+  <si>
+    <t>Cadastrar multas motorista</t>
+  </si>
+  <si>
+    <t>Cadastrar impostos do motorista</t>
+  </si>
+  <si>
+    <t>Cadastrar pedágios pagos pelo motorista</t>
+  </si>
+  <si>
+    <t>Cadastrar viajem, dando opção para os usuário do aplicativo peguem carona</t>
+  </si>
+  <si>
+    <t>usuário cadastrar viagens</t>
+  </si>
+  <si>
+    <t>Usuário cadastrar habastecimentos</t>
+  </si>
+  <si>
+    <t>Listar postos por recomendações</t>
+  </si>
+  <si>
+    <t>Mostrar se posto possui mecânico</t>
+  </si>
+  <si>
+    <t>Denunciar posto que não segue os preços apresentados</t>
+  </si>
+  <si>
+    <t>Filtrar postos por valor combustível</t>
+  </si>
+  <si>
+    <t>Gerar relatórios de consumo do carro mensalmente</t>
+  </si>
+  <si>
+    <t>Calcular e apresentar qual combustível é mais vantajoso para usuário, levando em conta o poder calorifico do motor ao etanlo é de 70% a gasolina</t>
+  </si>
+  <si>
+    <t>Informar a situação das vias de acordo com a rota traçada</t>
+  </si>
+  <si>
+    <t>Informar melhor rota de acordo com os postos mais baratos</t>
+  </si>
+  <si>
+    <t>Mostrar qual posto possui o melhor combustível na rota</t>
+  </si>
+  <si>
+    <t>Mostrar radares na rota</t>
+  </si>
+  <si>
+    <t>Mostrar pistas interditadas ( devido a acidentes, paralizações etc)</t>
+  </si>
+  <si>
+    <t>Motrar tempo restante da viagem</t>
+  </si>
+  <si>
+    <t>Fazer calculo pra ver se motorista consegue chegar no posto mais barato</t>
+  </si>
+  <si>
+    <t>Fazer calculo pra ver se o motorista consegue chegar no posto com a determinada bandeira</t>
+  </si>
+  <si>
+    <t>Faixa de idade dos entrevistados</t>
+  </si>
+  <si>
+    <t>Mostrar se posto possui loja de conveniencia, restaurantes e valores médios das refeições</t>
   </si>
 </sst>
 </file>
@@ -121,7 +301,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -156,6 +336,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -196,12 +379,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -209,14 +389,26 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="pt-BR"/>
+              <a:rPr lang="pt-BR" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
               <a:t>Valores da Gasolina Comum</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="pt-BR" baseline="0"/>
+              <a:rPr lang="pt-BR" b="1" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
               <a:t> em Santa Rita do Sapucaí-MG entre 06/01/2020 e 06/03/2020</a:t>
             </a:r>
-            <a:endParaRPr lang="pt-BR"/>
+            <a:endParaRPr lang="pt-BR" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
@@ -233,12 +425,9 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -1179,12 +1368,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -1242,10 +1428,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -1282,12 +1465,9 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -1356,12 +1536,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -1369,12 +1546,18 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="pt-BR" sz="1800" b="0" i="0" baseline="0">
+              <a:rPr lang="pt-BR" sz="1400" b="1" i="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
                 <a:effectLst/>
               </a:rPr>
               <a:t>Valores do Etanol em Santa Rita do Sapucaí-MG entre 06/01/2020 e 06/03/2020</a:t>
             </a:r>
-            <a:endParaRPr lang="pt-BR">
+            <a:endParaRPr lang="pt-BR" sz="1400" b="1" i="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
               <a:effectLst/>
             </a:endParaRPr>
           </a:p>
@@ -1393,12 +1576,9 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -2267,12 +2447,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -2328,12 +2505,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -2370,12 +2544,9 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -3905,8 +4076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F419A0E-6C88-4CD1-BCBF-61ABD01E164E}">
   <dimension ref="B2:Q46"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15:O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4782,36 +4953,513 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFBC412C-5268-4CB4-8635-53272D0623C4}">
-  <dimension ref="B2:C3"/>
+  <dimension ref="B1:D61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AS3" sqref="AS3"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.7109375" style="10"/>
-    <col min="2" max="3" width="30.7109375" style="10" customWidth="1"/>
-    <col min="4" max="16384" width="2.7109375" style="10"/>
+    <col min="2" max="2" width="60.7109375" style="10" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="2.7109375" style="10"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:4" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="11"/>
-    </row>
-    <row r="3" spans="2:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D2" s="11"/>
+    </row>
+    <row r="3" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B3" s="10" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>13</v>
       </c>
+      <c r="D3" s="10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B4" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="10">
+        <v>30</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B5" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="10">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B6" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" s="10">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B7" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="10">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B8" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B9" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B10" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B11" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B12" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B13" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B14" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B15" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B16" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B17" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B18" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B19" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B20" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B21" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B22" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B23" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B24" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B25" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B26" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B27" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B28" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B29" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B30" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B31" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C31" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B32" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C32" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B33" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C33" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B34" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C34" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B35" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C35" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B36" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C36" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B37" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C37" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B38" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C38" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B39" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C39" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B40" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C40" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B41" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C41" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B42" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C42" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B43" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C43" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B44" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C44" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B45" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C45" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B46" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C46" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B47" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C47" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B48" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C48" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B49" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C49" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B50" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C50" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B51" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C51" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B52" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C52" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B53" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C53" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B54" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="C54" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B55" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C55" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B56" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="C56" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B57" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="C57" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B58" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C58" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B59" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C59" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B60" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C60" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B61" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="C61" s="10">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:C61">
+    <sortCondition descending="1" ref="C4:C61"/>
+  </sortState>
   <mergeCells count="1">
-    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B2:D2"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>